<commit_message>
added some string programs
</commit_message>
<xml_diff>
--- a/List.xlsx
+++ b/List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arora\Desktop\Coding-Interview-101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24503CDA-7C62-4011-AF39-4D6907C4BC16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83A1CD4-4598-4ECB-83FB-C757B9D2C46A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="906">
   <si>
     <t>Topic:</t>
   </si>
@@ -2746,6 +2746,9 @@
   </si>
   <si>
     <t>do with min heaps too</t>
+  </si>
+  <si>
+    <t>check if s2 is substring of s1+s1 or not</t>
   </si>
 </sst>
 </file>
@@ -3192,8 +3195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3863,6 +3866,9 @@
       </c>
       <c r="C60" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="E60" t="s">
+        <v>905</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="21">

</xml_diff>